<commit_message>
Changes of 21st Sept 2022
</commit_message>
<xml_diff>
--- a/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult.xlsx
+++ b/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>FileName</t>
   </si>
@@ -65,156 +65,6 @@
   </si>
   <si>
     <t>FDXLoadTndr_1282020_189_19667476</t>
-  </si>
-  <si>
-    <t>32451272</t>
-  </si>
-  <si>
-    <t>32451273</t>
-  </si>
-  <si>
-    <t>32451274</t>
-  </si>
-  <si>
-    <t>32451275</t>
-  </si>
-  <si>
-    <t>32451276</t>
-  </si>
-  <si>
-    <t>32451277</t>
-  </si>
-  <si>
-    <t>32451278</t>
-  </si>
-  <si>
-    <t>32451279</t>
-  </si>
-  <si>
-    <t>32451280</t>
-  </si>
-  <si>
-    <t>32451281</t>
-  </si>
-  <si>
-    <t>32471821</t>
-  </si>
-  <si>
-    <t>32471822</t>
-  </si>
-  <si>
-    <t>32471823</t>
-  </si>
-  <si>
-    <t>32471824</t>
-  </si>
-  <si>
-    <t>32471825</t>
-  </si>
-  <si>
-    <t>32471826</t>
-  </si>
-  <si>
-    <t>32471827</t>
-  </si>
-  <si>
-    <t>32471828</t>
-  </si>
-  <si>
-    <t>32471829</t>
-  </si>
-  <si>
-    <t>32471830</t>
-  </si>
-  <si>
-    <t>32474736</t>
-  </si>
-  <si>
-    <t>32474737</t>
-  </si>
-  <si>
-    <t>32474738</t>
-  </si>
-  <si>
-    <t>32474739</t>
-  </si>
-  <si>
-    <t>32474740</t>
-  </si>
-  <si>
-    <t>32474741</t>
-  </si>
-  <si>
-    <t>32474742</t>
-  </si>
-  <si>
-    <t>32474743</t>
-  </si>
-  <si>
-    <t>32474744</t>
-  </si>
-  <si>
-    <t>32474745</t>
-  </si>
-  <si>
-    <t>32476809</t>
-  </si>
-  <si>
-    <t>32476810</t>
-  </si>
-  <si>
-    <t>32476811</t>
-  </si>
-  <si>
-    <t>32476812</t>
-  </si>
-  <si>
-    <t>32476813</t>
-  </si>
-  <si>
-    <t>32476817</t>
-  </si>
-  <si>
-    <t>32476819</t>
-  </si>
-  <si>
-    <t>32476820</t>
-  </si>
-  <si>
-    <t>32476821</t>
-  </si>
-  <si>
-    <t>32476822</t>
-  </si>
-  <si>
-    <t>32482898</t>
-  </si>
-  <si>
-    <t>32482899</t>
-  </si>
-  <si>
-    <t>32482900</t>
-  </si>
-  <si>
-    <t>32482901</t>
-  </si>
-  <si>
-    <t>32482902</t>
-  </si>
-  <si>
-    <t>32482903</t>
-  </si>
-  <si>
-    <t>32482904</t>
-  </si>
-  <si>
-    <t>32482905</t>
-  </si>
-  <si>
-    <t>32482906</t>
-  </si>
-  <si>
-    <t>32482907</t>
   </si>
   <si>
     <t>32483151</t>
@@ -251,7 +101,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -600,13 +449,13 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -621,80 +470,80 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>67</v>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>69</v>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>70</v>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>71</v>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>72</v>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>73</v>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>74</v>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>75</v>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>76</v>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
Changes of CPU and H3P service
</commit_message>
<xml_diff>
--- a/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult.xlsx
+++ b/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FileName</t>
   </si>
@@ -34,39 +34,6 @@
     <t>FDXLoadTndr_1272020_216_19663511</t>
   </si>
   <si>
-    <t>FDXLoadTndr_1272020_1918_19663362</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1956_19667650</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1932_19667611</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1925_19667593</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1855_19667541</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1855_19667542</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1845_19667530</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_1824_19667472</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_189_19667475</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_189_19667468</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1282020_189_19667476</t>
-  </si>
-  <si>
     <t>32483151</t>
   </si>
   <si>
@@ -79,22 +46,7 @@
     <t>32483154</t>
   </si>
   <si>
-    <t>32483155</t>
-  </si>
-  <si>
-    <t>32483156</t>
-  </si>
-  <si>
-    <t>32483157</t>
-  </si>
-  <si>
-    <t>32483158</t>
-  </si>
-  <si>
-    <t>32483159</t>
-  </si>
-  <si>
-    <t>32483160</t>
+    <t>Service</t>
   </si>
 </sst>
 </file>
@@ -107,12 +59,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -142,9 +100,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,123 +421,52 @@
     <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1"/>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>